<commit_message>
csv writer + some refactoring
</commit_message>
<xml_diff>
--- a/reader.xlsx
+++ b/reader.xlsx
@@ -5,14 +5,14 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleb/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleb/PycharmProjects/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -23,14 +23,159 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t xml:space="preserve">  http://www.mazda.genser.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-asc.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-bcrmotors.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-elkemotor.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-kaluga.genser.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazdanv.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-sibautocentr.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mazda-yaroslavl.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-asmoto.ru  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-astrakhan.ru/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-autoforum.ru  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-avangard.ru  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-irkutsk.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-izmaylovo.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-kama.ru/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.mercedes-khabarovsk.ru</t>
+  </si>
+  <si>
+    <t>скидка</t>
+  </si>
+  <si>
+    <t>акция</t>
+  </si>
+  <si>
+    <t>подарок</t>
+  </si>
+  <si>
+    <t>специальная цена</t>
+  </si>
+  <si>
+    <t>Спецпредложения</t>
+  </si>
+  <si>
+    <t>уникальны</t>
+  </si>
+  <si>
+    <t>специальн предложен</t>
+  </si>
+  <si>
+    <t>выгод</t>
+  </si>
+  <si>
+    <t>эксклюзивн услови</t>
+  </si>
+  <si>
+    <t>преимуществ</t>
+  </si>
+  <si>
+    <t>уникальн цен</t>
+  </si>
+  <si>
+    <t>привлекательн услови</t>
+  </si>
+  <si>
+    <t>кампани</t>
+  </si>
+  <si>
+    <t>дари</t>
+  </si>
+  <si>
+    <t>предлага услуг</t>
+  </si>
+  <si>
+    <t>привилеги</t>
+  </si>
+  <si>
+    <t>рекордн услови</t>
+  </si>
+  <si>
+    <t>комплимент</t>
+  </si>
+  <si>
+    <t>услови</t>
+  </si>
+  <si>
+    <t>предложен ограничен</t>
+  </si>
+  <si>
+    <t>наш клиент</t>
+  </si>
+  <si>
+    <t>распродажа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">успей </t>
+  </si>
+  <si>
+    <t>сейчас или никогда</t>
+  </si>
+  <si>
+    <t>предложен дня</t>
+  </si>
+  <si>
+    <t>только сейчас</t>
+  </si>
+  <si>
+    <t>только сегодн</t>
+  </si>
+  <si>
+    <t>гарантия лучшей цены</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -54,8 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -333,12 +479,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>